<commit_message>
test append of data
</commit_message>
<xml_diff>
--- a/books.xlsx
+++ b/books.xlsx
@@ -375,7 +375,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
@@ -397,6 +397,116 @@
       <c r="C1" s="2" t="inlineStr">
         <is>
           <t>class</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="n">
+        <v>88</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>46</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="n">
+        <v>89</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>38</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>59</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="n">
+        <v>56</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="n">
+        <v>34</v>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>type1</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>type2</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="inlineStr">
+        <is>
+          <t>type3</t>
+        </is>
+      </c>
+      <c r="D8" s="2" t="inlineStr">
+        <is>
+          <t>type4</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>tup1</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>tup2</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>tup3</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>tup4</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
2 logo added everything else aligned, still there's a room for improvement
</commit_message>
<xml_diff>
--- a/books.xlsx
+++ b/books.xlsx
@@ -375,7 +375,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
@@ -507,6 +507,357 @@
       <c r="D9" s="2" t="inlineStr">
         <is>
           <t>tup4</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>mewa</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="inlineStr">
+        <is>
+          <t>language</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="inlineStr">
+        <is>
+          <t>mewa</t>
+        </is>
+      </c>
+      <c r="D10" s="2" t="inlineStr">
+        <is>
+          <t>acmom</t>
+        </is>
+      </c>
+      <c r="E10" s="2" t="inlineStr">
+        <is>
+          <t>400 - mew</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="inlineStr">
+        <is>
+          <t>english</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="inlineStr">
+        <is>
+          <t>language</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="inlineStr">
+        <is>
+          <t>mewa</t>
+        </is>
+      </c>
+      <c r="D11" s="2" t="inlineStr">
+        <is>
+          <t>englis</t>
+        </is>
+      </c>
+      <c r="E11" s="2" t="inlineStr">
+        <is>
+          <t>400 - mew</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="inlineStr">
+        <is>
+          <t>arabic</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="inlineStr">
+        <is>
+          <t>arts</t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="inlineStr">
+        <is>
+          <t>mombasa</t>
+        </is>
+      </c>
+      <c r="D12" s="2" t="inlineStr">
+        <is>
+          <t>county</t>
+        </is>
+      </c>
+      <c r="E12" s="2" t="inlineStr">
+        <is>
+          <t>700 - mom</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="inlineStr">
+        <is>
+          <t>the sun also rises</t>
+        </is>
+      </c>
+      <c r="B13" s="2" t="inlineStr">
+        <is>
+          <t>language</t>
+        </is>
+      </c>
+      <c r="C13" s="2" t="inlineStr">
+        <is>
+          <t>hemingway</t>
+        </is>
+      </c>
+      <c r="D13" s="2" t="inlineStr">
+        <is>
+          <t>hemingway</t>
+        </is>
+      </c>
+      <c r="E13" s="2" t="inlineStr">
+        <is>
+          <t>400 - hem</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>sentender</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="inlineStr">
+        <is>
+          <t>language</t>
+        </is>
+      </c>
+      <c r="C14" s="2" t="inlineStr">
+        <is>
+          <t>emanuela</t>
+        </is>
+      </c>
+      <c r="D14" s="2" t="inlineStr">
+        <is>
+          <t>mark</t>
+        </is>
+      </c>
+      <c r="E14" s="2" t="inlineStr">
+        <is>
+          <t>400 - ema</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="inlineStr">
+        <is>
+          <t>english</t>
+        </is>
+      </c>
+      <c r="B15" s="2" t="inlineStr">
+        <is>
+          <t>language</t>
+        </is>
+      </c>
+      <c r="C15" s="2" t="inlineStr">
+        <is>
+          <t>samuel</t>
+        </is>
+      </c>
+      <c r="D15" s="2" t="inlineStr">
+        <is>
+          <t>etoo</t>
+        </is>
+      </c>
+      <c r="E15" s="2" t="inlineStr">
+        <is>
+          <t>400 - sam</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="inlineStr">
+        <is>
+          <t>english</t>
+        </is>
+      </c>
+      <c r="B16" s="2" t="inlineStr">
+        <is>
+          <t>language</t>
+        </is>
+      </c>
+      <c r="C16" s="2" t="inlineStr">
+        <is>
+          <t>arab</t>
+        </is>
+      </c>
+      <c r="D16" s="2" t="inlineStr">
+        <is>
+          <t>english</t>
+        </is>
+      </c>
+      <c r="E16" s="2" t="inlineStr">
+        <is>
+          <t>400 - ara</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="inlineStr">
+        <is>
+          <t>english</t>
+        </is>
+      </c>
+      <c r="B17" s="2" t="inlineStr">
+        <is>
+          <t>language</t>
+        </is>
+      </c>
+      <c r="C17" s="2" t="inlineStr">
+        <is>
+          <t>ann</t>
+        </is>
+      </c>
+      <c r="D17" s="2" t="inlineStr">
+        <is>
+          <t>etoo</t>
+        </is>
+      </c>
+      <c r="E17" s="2" t="inlineStr">
+        <is>
+          <t>400 - ann</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="inlineStr">
+        <is>
+          <t>english</t>
+        </is>
+      </c>
+      <c r="B18" s="2" t="inlineStr">
+        <is>
+          <t>language</t>
+        </is>
+      </c>
+      <c r="C18" s="2" t="inlineStr">
+        <is>
+          <t>ann</t>
+        </is>
+      </c>
+      <c r="D18" s="2" t="inlineStr">
+        <is>
+          <t>etoo</t>
+        </is>
+      </c>
+      <c r="E18" s="2" t="inlineStr">
+        <is>
+          <t>400 - ann</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="inlineStr">
+        <is>
+          <t>english</t>
+        </is>
+      </c>
+      <c r="B19" s="2" t="inlineStr">
+        <is>
+          <t>language</t>
+        </is>
+      </c>
+      <c r="C19" s="2" t="inlineStr">
+        <is>
+          <t>ann</t>
+        </is>
+      </c>
+      <c r="D19" s="2" t="inlineStr">
+        <is>
+          <t>etoo</t>
+        </is>
+      </c>
+      <c r="E19" s="2" t="inlineStr">
+        <is>
+          <t>400 - ann</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="inlineStr">
+        <is>
+          <t>english</t>
+        </is>
+      </c>
+      <c r="B20" s="2" t="inlineStr">
+        <is>
+          <t>language</t>
+        </is>
+      </c>
+      <c r="C20" s="2" t="inlineStr">
+        <is>
+          <t>ann</t>
+        </is>
+      </c>
+      <c r="D20" s="2" t="inlineStr">
+        <is>
+          <t>etoo</t>
+        </is>
+      </c>
+      <c r="E20" s="2" t="inlineStr">
+        <is>
+          <t>400 - ann</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>english</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>language</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>ann</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>etoo</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>400 - ann</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>mathe</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>language</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>engli</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>ann</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>400 - eng</t>
         </is>
       </c>
     </row>

</xml_diff>